<commit_message>
Updated the GUI.excel_output to close when the crawling starts.
</commit_message>
<xml_diff>
--- a/data/data_table.xlsx
+++ b/data/data_table.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>Credit_(GBP)</t>
   </si>
@@ -34,61 +34,46 @@
     <t>Working Professional</t>
   </si>
   <si>
-    <t>AC-BCE59E</t>
-  </si>
-  <si>
-    <t>AZ-F963FD</t>
-  </si>
-  <si>
-    <t>DA-CA4035</t>
-  </si>
-  <si>
-    <t>HG-DA9892</t>
-  </si>
-  <si>
-    <t>IW-0AF3A0</t>
-  </si>
-  <si>
-    <t>JK-0AF3B3</t>
-  </si>
-  <si>
-    <t>KM-6187CE</t>
-  </si>
-  <si>
-    <t>KO-5A2A3E</t>
-  </si>
-  <si>
-    <t>NS-1032D4</t>
-  </si>
-  <si>
-    <t>PM-629971</t>
-  </si>
-  <si>
-    <t>RF-D6BC4E</t>
-  </si>
-  <si>
-    <t>RI-938451</t>
-  </si>
-  <si>
-    <t>SM-3362BB</t>
-  </si>
-  <si>
-    <t>AG-6FF196</t>
-  </si>
-  <si>
-    <t>KM-6FFC6E</t>
-  </si>
-  <si>
-    <t>MD-D6BC86</t>
-  </si>
-  <si>
-    <t>18-06-2021</t>
-  </si>
-  <si>
-    <t>19-06-2021</t>
-  </si>
-  <si>
-    <t>20-06-2021</t>
+    <t>AS-CB728C</t>
+  </si>
+  <si>
+    <t>CA-CB49D4</t>
+  </si>
+  <si>
+    <t>CG-5EB883</t>
+  </si>
+  <si>
+    <t>CG-CB74ED</t>
+  </si>
+  <si>
+    <t>CL-BE26EF</t>
+  </si>
+  <si>
+    <t>GH-FE0E73</t>
+  </si>
+  <si>
+    <t>IM-74682B</t>
+  </si>
+  <si>
+    <t>JE-CB64CF</t>
+  </si>
+  <si>
+    <t>MS-CB7818</t>
+  </si>
+  <si>
+    <t>RB-5EEEF0</t>
+  </si>
+  <si>
+    <t>SR-3F1063</t>
+  </si>
+  <si>
+    <t>YW-0DA6F3</t>
+  </si>
+  <si>
+    <t>RA-044F6A</t>
+  </si>
+  <si>
+    <t>22-07-2021</t>
   </si>
 </sst>
 </file>
@@ -446,7 +431,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -477,13 +462,13 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D2">
-        <v>308.64</v>
+        <v>391.04</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -492,10 +477,10 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D3">
-        <v>731.3599999999999</v>
+        <v>690</v>
       </c>
       <c r="E3">
         <v>8</v>
@@ -507,13 +492,13 @@
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D4">
-        <v>450</v>
+        <v>443.44</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -522,10 +507,10 @@
         <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D5">
-        <v>295</v>
+        <v>461.14</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -537,10 +522,10 @@
         <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D6">
-        <v>295</v>
+        <v>311.76</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -552,13 +537,13 @@
         <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D7">
-        <v>427.6</v>
+        <v>295</v>
       </c>
       <c r="E7">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -567,13 +552,13 @@
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D8">
-        <v>436.46</v>
+        <v>404.8000000000001</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -582,13 +567,13 @@
         <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D9">
-        <v>417.6</v>
+        <v>398.4</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -597,13 +582,13 @@
         <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D10">
-        <v>225</v>
+        <v>436.16</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -612,13 +597,13 @@
         <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D11">
-        <v>685.3599999999999</v>
+        <v>478.69</v>
       </c>
       <c r="E11">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -627,10 +612,10 @@
         <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D12">
-        <v>460</v>
+        <v>347.76</v>
       </c>
       <c r="E12">
         <v>8</v>
@@ -642,81 +627,35 @@
         <v>17</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D13">
-        <v>358.74</v>
+        <v>658.16</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D14">
-        <v>364</v>
+        <v>977.5200000000002</v>
       </c>
       <c r="E14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15">
-        <v>750</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16">
-        <v>1144.2</v>
-      </c>
-      <c r="E16">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17">
-        <v>1610</v>
-      </c>
-      <c r="E17">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:A14"/>
-    <mergeCell ref="A15:A17"/>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>